<commit_message>
Qualitative data on political stability
</commit_message>
<xml_diff>
--- a/qualitativeData/data on political stability/List of African countries - Data collection.xlsx
+++ b/qualitativeData/data on political stability/List of African countries - Data collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratsi\Dropbox\AFRICAN POLITICS RESEARCH\ELUSIVE QUEST\qualitativeData\data on political stability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11A79889-099A-478C-8BDF-C89CBAC69DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108DA597-0B49-4FF4-B7F1-14506CFDA6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ACD109BA-B679-4F5C-A370-91BA12290E79}"/>
   </bookViews>
@@ -255,12 +255,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -298,13 +304,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1DA9A8-7600-42E3-8F30-3B5B16251F74}">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -632,10 +638,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>55</v>
       </c>
     </row>
@@ -643,325 +649,325 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="7"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="7"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="7"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="5"/>
+      <c r="B27" s="7"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="7"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" s="7"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="7"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="5"/>
+      <c r="B34" s="7"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="5"/>
+      <c r="B35" s="7"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="5"/>
+      <c r="B36" s="7"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="5"/>
+      <c r="B37" s="7"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="5"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="5"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="5"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="5"/>
+      <c r="B41" s="7"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="5"/>
+      <c r="B42" s="7"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="5"/>
+      <c r="B43" s="7"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="5"/>
+      <c r="B44" s="7"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="5"/>
+      <c r="B45" s="7"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="5"/>
+      <c r="B46" s="7"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="5"/>
+      <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="5"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="5"/>
+      <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="5"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="5"/>
+      <c r="B51" s="7"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="5"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="5"/>
+      <c r="B53" s="7"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="5"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="5"/>
+      <c r="B55" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>